<commit_message>
Change column name from "name" to "owner"
</commit_message>
<xml_diff>
--- a/FFData_Sep5.xlsx
+++ b/FFData_Sep5.xlsx
@@ -200,9 +200,6 @@
     <t>CrackerDeezNutz</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Jose</t>
   </si>
   <si>
@@ -609,6 +606,9 @@
   </si>
   <si>
     <t>Top 3 Finish</t>
+  </si>
+  <si>
+    <t>Owner</t>
   </si>
 </sst>
 </file>
@@ -1002,9 +1002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1019,16 +1017,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>178</v>
       </c>
-      <c r="D1" t="s">
-        <v>179</v>
-      </c>
       <c r="E1" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1076,7 +1074,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>39</v>
@@ -1104,16 +1102,16 @@
         <v>2008</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1121,16 +1119,16 @@
         <v>2009</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1138,16 +1136,16 @@
         <v>2010</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1155,16 +1153,16 @@
         <v>2011</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
         <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1172,16 +1170,16 @@
         <v>2012</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
         <v>115</v>
       </c>
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" t="s">
-        <v>116</v>
-      </c>
       <c r="E10" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1189,16 +1187,16 @@
         <v>2013</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
         <v>124</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>125</v>
       </c>
-      <c r="D11" t="s">
-        <v>126</v>
-      </c>
       <c r="E11" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1206,16 +1204,16 @@
         <v>2014</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" t="s">
         <v>139</v>
       </c>
-      <c r="C12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D12" t="s">
-        <v>140</v>
-      </c>
       <c r="E12" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1223,16 +1221,16 @@
         <v>2015</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="D13" t="s">
-        <v>153</v>
-      </c>
       <c r="E13" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1240,16 +1238,16 @@
         <v>2016</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1280,10 +1278,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,7 +1348,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>25</v>
@@ -1381,7 +1379,7 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1451,7 +1449,7 @@
         <v>49</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,10 +1460,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1476,10 +1474,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1493,7 +1491,7 @@
         <v>48</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1504,10 +1502,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1521,7 +1519,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1535,7 +1533,7 @@
         <v>49</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1546,10 +1544,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1560,10 +1558,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1577,7 +1575,7 @@
         <v>11</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1591,7 +1589,7 @@
         <v>49</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1605,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1630,10 +1628,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1647,7 +1645,7 @@
         <v>11</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1658,10 +1656,10 @@
         <v>3</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1672,10 +1670,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>125</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1686,10 +1684,10 @@
         <v>2</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1700,10 +1698,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1714,10 +1712,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1728,10 +1726,10 @@
         <v>2</v>
       </c>
       <c r="C33" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>125</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1745,7 +1743,7 @@
         <v>48</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,10 +1754,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1770,10 +1768,10 @@
         <v>2</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1784,10 +1782,10 @@
         <v>3</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1798,10 +1796,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1812,10 +1810,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1826,10 +1824,10 @@
         <v>3</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1856,10 +1854,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2002,7 +2000,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2035,7 +2033,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2046,7 +2044,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2057,7 +2055,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2068,7 +2066,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2079,7 +2077,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2090,7 +2088,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2101,7 +2099,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2112,7 +2110,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2123,7 +2121,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2134,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2145,7 +2143,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2156,7 +2154,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2167,7 +2165,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2178,7 +2176,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2189,7 +2187,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2200,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2211,7 +2209,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2222,7 +2220,7 @@
         <v>3</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2233,7 +2231,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2244,7 +2242,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2255,7 +2253,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2266,7 +2264,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2277,7 +2275,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2288,7 +2286,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2318,34 +2316,34 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>193</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
@@ -2357,10 +2355,10 @@
         <v>14</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>4</v>
@@ -2369,7 +2367,7 @@
         <v>29</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -2396,11 +2394,11 @@
         <v>201</v>
       </c>
       <c r="H2" s="14">
-        <f>E2/SUM($L2:$N2)</f>
+        <f t="shared" ref="H2:I5" si="0">E2/SUM($L2:$N2)</f>
         <v>88.647058823529406</v>
       </c>
       <c r="I2" s="14">
-        <f>F2/SUM($L2:$N2)</f>
+        <f t="shared" si="0"/>
         <v>76.82352941176471</v>
       </c>
       <c r="J2" s="14">
@@ -2452,15 +2450,15 @@
         <v>1076</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G5" si="0">E3-F3</f>
+        <f t="shared" ref="G3:G5" si="1">E3-F3</f>
         <v>0</v>
       </c>
       <c r="H3" s="14">
-        <f>E3/SUM($L3:$N3)</f>
+        <f t="shared" si="0"/>
         <v>82.769230769230774</v>
       </c>
       <c r="I3" s="14">
-        <f>F3/SUM($L3:$N3)</f>
+        <f t="shared" si="0"/>
         <v>82.769230769230774</v>
       </c>
       <c r="J3" s="14">
@@ -2500,7 +2498,7 @@
         <v>2006</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>42</v>
@@ -2512,15 +2510,15 @@
         <v>1463</v>
       </c>
       <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>-211</v>
+      </c>
+      <c r="H4" s="14">
         <f t="shared" si="0"/>
-        <v>-211</v>
-      </c>
-      <c r="H4" s="14">
-        <f>E4/SUM($L4:$N4)</f>
         <v>96.307692307692307</v>
       </c>
       <c r="I4" s="14">
-        <f>F4/SUM($L4:$N4)</f>
+        <f t="shared" si="0"/>
         <v>112.53846153846153</v>
       </c>
       <c r="J4" s="14">
@@ -2560,7 +2558,7 @@
         <v>2007</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>51</v>
@@ -2572,15 +2570,15 @@
         <v>1474</v>
       </c>
       <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>-298</v>
+      </c>
+      <c r="H5" s="14">
         <f t="shared" si="0"/>
-        <v>-298</v>
-      </c>
-      <c r="H5" s="14">
-        <f>E5/SUM($L5:$N5)</f>
         <v>90.461538461538467</v>
       </c>
       <c r="I5" s="14">
-        <f>F5/SUM($L5:$N5)</f>
+        <f t="shared" si="0"/>
         <v>113.38461538461539</v>
       </c>
       <c r="J5" s="14">
@@ -2620,10 +2618,10 @@
         <v>2008</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="1">
         <v>1264</v>
@@ -2636,15 +2634,15 @@
         <v>-41</v>
       </c>
       <c r="H6" s="14">
-        <f t="shared" ref="H6:H66" si="1">E6/SUM($L6:$N6)</f>
+        <f t="shared" ref="H6:H66" si="2">E6/SUM($L6:$N6)</f>
         <v>97.230769230769226</v>
       </c>
       <c r="I6" s="14">
-        <f t="shared" ref="I6:I66" si="2">F6/SUM($L6:$N6)</f>
+        <f t="shared" ref="I6:I66" si="3">F6/SUM($L6:$N6)</f>
         <v>100.38461538461539</v>
       </c>
       <c r="J6" s="14">
-        <f t="shared" ref="J6:J66" si="3">H6-I6</f>
+        <f t="shared" ref="J6:J66" si="4">H6-I6</f>
         <v>-3.1538461538461604</v>
       </c>
       <c r="K6" s="1">
@@ -2680,7 +2678,7 @@
         <v>2009</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>7</v>
@@ -2696,15 +2694,15 @@
         <v>-56</v>
       </c>
       <c r="H7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116.84615384615384</v>
       </c>
       <c r="I7" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121.15384615384616</v>
       </c>
       <c r="J7" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.3076923076923208</v>
       </c>
       <c r="K7" s="1">
@@ -2740,10 +2738,10 @@
         <v>2010</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" s="1">
         <v>1527</v>
@@ -2756,15 +2754,15 @@
         <v>150</v>
       </c>
       <c r="H8" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>117.46153846153847</v>
       </c>
       <c r="I8" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105.92307692307692</v>
       </c>
       <c r="J8" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.538461538461547</v>
       </c>
       <c r="K8" s="1">
@@ -2800,10 +2798,10 @@
         <v>2011</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="1">
         <v>1565</v>
@@ -2816,15 +2814,15 @@
         <v>40</v>
       </c>
       <c r="H9" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120.38461538461539</v>
       </c>
       <c r="I9" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117.30769230769231</v>
       </c>
       <c r="J9" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.0769230769230802</v>
       </c>
       <c r="K9" s="1">
@@ -2860,10 +2858,10 @@
         <v>2012</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E10" s="1">
         <v>1387</v>
@@ -2872,19 +2870,19 @@
         <v>1358</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" ref="G10:G14" si="4">E10-F10</f>
+        <f t="shared" ref="G10:G14" si="5">E10-F10</f>
         <v>29</v>
       </c>
       <c r="H10" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106.69230769230769</v>
       </c>
       <c r="I10" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104.46153846153847</v>
       </c>
       <c r="J10" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2307692307692264</v>
       </c>
       <c r="K10" s="1">
@@ -2920,10 +2918,10 @@
         <v>2013</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E11" s="1">
         <v>1519</v>
@@ -2932,19 +2930,19 @@
         <v>1359</v>
       </c>
       <c r="G11" s="1">
+        <f t="shared" si="5"/>
+        <v>160</v>
+      </c>
+      <c r="H11" s="14">
+        <f t="shared" si="2"/>
+        <v>116.84615384615384</v>
+      </c>
+      <c r="I11" s="14">
+        <f t="shared" si="3"/>
+        <v>104.53846153846153</v>
+      </c>
+      <c r="J11" s="14">
         <f t="shared" si="4"/>
-        <v>160</v>
-      </c>
-      <c r="H11" s="14">
-        <f t="shared" si="1"/>
-        <v>116.84615384615384</v>
-      </c>
-      <c r="I11" s="14">
-        <f t="shared" si="2"/>
-        <v>104.53846153846153</v>
-      </c>
-      <c r="J11" s="14">
-        <f t="shared" si="3"/>
         <v>12.307692307692307</v>
       </c>
       <c r="K11" s="1">
@@ -2980,10 +2978,10 @@
         <v>2014</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" s="1">
         <v>1443</v>
@@ -2992,19 +2990,19 @@
         <v>1476</v>
       </c>
       <c r="G12" s="1">
+        <f t="shared" si="5"/>
+        <v>-33</v>
+      </c>
+      <c r="H12" s="14">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="I12" s="14">
+        <f t="shared" si="3"/>
+        <v>113.53846153846153</v>
+      </c>
+      <c r="J12" s="14">
         <f t="shared" si="4"/>
-        <v>-33</v>
-      </c>
-      <c r="H12" s="14">
-        <f t="shared" si="1"/>
-        <v>111</v>
-      </c>
-      <c r="I12" s="14">
-        <f t="shared" si="2"/>
-        <v>113.53846153846153</v>
-      </c>
-      <c r="J12" s="14">
-        <f t="shared" si="3"/>
         <v>-2.538461538461533</v>
       </c>
       <c r="K12" s="1">
@@ -3040,10 +3038,10 @@
         <v>2015</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E13" s="1">
         <v>1307</v>
@@ -3052,19 +3050,19 @@
         <v>1474</v>
       </c>
       <c r="G13" s="1">
+        <f t="shared" si="5"/>
+        <v>-167</v>
+      </c>
+      <c r="H13" s="14">
+        <f t="shared" si="2"/>
+        <v>100.53846153846153</v>
+      </c>
+      <c r="I13" s="14">
+        <f t="shared" si="3"/>
+        <v>113.38461538461539</v>
+      </c>
+      <c r="J13" s="14">
         <f t="shared" si="4"/>
-        <v>-167</v>
-      </c>
-      <c r="H13" s="14">
-        <f t="shared" si="1"/>
-        <v>100.53846153846153</v>
-      </c>
-      <c r="I13" s="14">
-        <f t="shared" si="2"/>
-        <v>113.38461538461539</v>
-      </c>
-      <c r="J13" s="14">
-        <f t="shared" si="3"/>
         <v>-12.846153846153854</v>
       </c>
       <c r="K13" s="1">
@@ -3100,10 +3098,10 @@
         <v>2016</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E14" s="1">
         <v>1460</v>
@@ -3112,19 +3110,19 @@
         <v>1486</v>
       </c>
       <c r="G14" s="1">
+        <f t="shared" si="5"/>
+        <v>-26</v>
+      </c>
+      <c r="H14" s="14">
+        <f t="shared" si="2"/>
+        <v>112.30769230769231</v>
+      </c>
+      <c r="I14" s="14">
+        <f t="shared" si="3"/>
+        <v>114.30769230769231</v>
+      </c>
+      <c r="J14" s="14">
         <f t="shared" si="4"/>
-        <v>-26</v>
-      </c>
-      <c r="H14" s="14">
-        <f t="shared" si="1"/>
-        <v>112.30769230769231</v>
-      </c>
-      <c r="I14" s="14">
-        <f t="shared" si="2"/>
-        <v>114.30769230769231</v>
-      </c>
-      <c r="J14" s="14">
-        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
       <c r="K14" s="1">
@@ -3160,7 +3158,7 @@
         <v>2004</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
@@ -3176,15 +3174,15 @@
         <v>120</v>
       </c>
       <c r="H15" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>86.705882352941174</v>
       </c>
       <c r="I15" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79.647058823529406</v>
       </c>
       <c r="J15" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.058823529411768</v>
       </c>
       <c r="K15" s="1">
@@ -3232,19 +3230,19 @@
         <v>1046</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" ref="G16:G21" si="5">E16-F16</f>
+        <f t="shared" ref="G16:G21" si="6">E16-F16</f>
         <v>-66</v>
       </c>
       <c r="H16" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75.384615384615387</v>
       </c>
       <c r="I16" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80.461538461538467</v>
       </c>
       <c r="J16" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-5.0769230769230802</v>
       </c>
       <c r="K16" s="1">
@@ -3280,7 +3278,7 @@
         <v>2006</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>24</v>
@@ -3292,19 +3290,19 @@
         <v>1343</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-34</v>
       </c>
       <c r="H17" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100.69230769230769</v>
       </c>
       <c r="I17" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>103.30769230769231</v>
       </c>
       <c r="J17" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.6153846153846132</v>
       </c>
       <c r="K17" s="1">
@@ -3352,19 +3350,19 @@
         <v>1471</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="H18" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118.07692307692308</v>
       </c>
       <c r="I18" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113.15384615384616</v>
       </c>
       <c r="J18" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.9230769230769198</v>
       </c>
       <c r="K18" s="1">
@@ -3400,10 +3398,10 @@
         <v>2008</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="1">
         <v>1453</v>
@@ -3412,19 +3410,19 @@
         <v>1322</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>131</v>
       </c>
       <c r="H19" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111.76923076923077</v>
       </c>
       <c r="I19" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101.69230769230769</v>
       </c>
       <c r="J19" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.07692307692308</v>
       </c>
       <c r="K19" s="1">
@@ -3460,10 +3458,10 @@
         <v>2009</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="E20" s="1">
         <v>1643</v>
@@ -3472,19 +3470,19 @@
         <v>1526</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>117</v>
       </c>
       <c r="H20" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>126.38461538461539</v>
       </c>
       <c r="I20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117.38461538461539</v>
       </c>
       <c r="J20" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="K20" s="1">
@@ -3520,10 +3518,10 @@
         <v>2010</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E21" s="1">
         <v>1592</v>
@@ -3532,19 +3530,19 @@
         <v>1386</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>206</v>
       </c>
       <c r="H21" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>122.46153846153847</v>
       </c>
       <c r="I21" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106.61538461538461</v>
       </c>
       <c r="J21" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.846153846153854</v>
       </c>
       <c r="K21" s="1">
@@ -3583,7 +3581,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" s="1">
         <v>1562</v>
@@ -3592,19 +3590,19 @@
         <v>1419</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" ref="G22:G27" si="6">E22-F22</f>
+        <f t="shared" ref="G22:G27" si="7">E22-F22</f>
         <v>143</v>
       </c>
       <c r="H22" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120.15384615384616</v>
       </c>
       <c r="I22" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109.15384615384616</v>
       </c>
       <c r="J22" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="K22" s="1">
@@ -3640,10 +3638,10 @@
         <v>2012</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E23" s="1">
         <v>1364</v>
@@ -3652,19 +3650,19 @@
         <v>1593</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-229</v>
       </c>
       <c r="H23" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104.92307692307692</v>
       </c>
       <c r="I23" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122.53846153846153</v>
       </c>
       <c r="J23" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-17.615384615384613</v>
       </c>
       <c r="K23" s="1">
@@ -3700,10 +3698,10 @@
         <v>2013</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" s="1">
         <v>1532</v>
@@ -3712,19 +3710,19 @@
         <v>1665</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-133</v>
       </c>
       <c r="H24" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>117.84615384615384</v>
       </c>
       <c r="I24" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>128.07692307692307</v>
       </c>
       <c r="J24" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-10.230769230769226</v>
       </c>
       <c r="K24" s="1">
@@ -3760,10 +3758,10 @@
         <v>2014</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E25" s="1">
         <v>1750</v>
@@ -3772,19 +3770,19 @@
         <v>1495</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>255</v>
       </c>
       <c r="H25" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>134.61538461538461</v>
       </c>
       <c r="I25" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115</v>
       </c>
       <c r="J25" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19.615384615384613</v>
       </c>
       <c r="K25" s="1">
@@ -3820,10 +3818,10 @@
         <v>2015</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E26" s="1">
         <v>1554</v>
@@ -3832,19 +3830,19 @@
         <v>1537</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="H26" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119.53846153846153</v>
       </c>
       <c r="I26" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>118.23076923076923</v>
       </c>
       <c r="J26" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3076923076923066</v>
       </c>
       <c r="K26" s="1">
@@ -3880,10 +3878,10 @@
         <v>2016</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E27" s="1">
         <v>1442</v>
@@ -3892,19 +3890,19 @@
         <v>1618</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-176</v>
       </c>
       <c r="H27" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110.92307692307692</v>
       </c>
       <c r="I27" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>124.46153846153847</v>
       </c>
       <c r="J27" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-13.538461538461547</v>
       </c>
       <c r="K27" s="1">
@@ -3934,7 +3932,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1">
         <v>2004</v>
@@ -3956,15 +3954,15 @@
         <v>-102</v>
       </c>
       <c r="H28" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>73.470588235294116</v>
       </c>
       <c r="I28" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79.470588235294116</v>
       </c>
       <c r="J28" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-6</v>
       </c>
       <c r="K28" s="1">
@@ -3994,7 +3992,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1">
         <v>2005</v>
@@ -4012,19 +4010,19 @@
         <v>1011</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" ref="G29:G34" si="7">E29-F29</f>
+        <f t="shared" ref="G29:G34" si="8">E29-F29</f>
         <v>-51</v>
       </c>
       <c r="H29" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>73.84615384615384</v>
       </c>
       <c r="I29" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77.769230769230774</v>
       </c>
       <c r="J29" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3.923076923076934</v>
       </c>
       <c r="K29" s="1">
@@ -4054,7 +4052,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1">
         <v>2006</v>
@@ -4072,19 +4070,19 @@
         <v>1458</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-149</v>
       </c>
       <c r="H30" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100.69230769230769</v>
       </c>
       <c r="I30" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>112.15384615384616</v>
       </c>
       <c r="J30" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-11.461538461538467</v>
       </c>
       <c r="K30" s="1">
@@ -4114,7 +4112,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1">
         <v>2007</v>
@@ -4132,19 +4130,19 @@
         <v>1353</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>83</v>
       </c>
       <c r="H31" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110.46153846153847</v>
       </c>
       <c r="I31" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104.07692307692308</v>
       </c>
       <c r="J31" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.3846153846153868</v>
       </c>
       <c r="K31" s="1">
@@ -4174,13 +4172,13 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" s="1">
         <v>2008</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>55</v>
@@ -4192,19 +4190,19 @@
         <v>1246</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>296</v>
       </c>
       <c r="H32" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118.61538461538461</v>
       </c>
       <c r="I32" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>95.84615384615384</v>
       </c>
       <c r="J32" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22.769230769230774</v>
       </c>
       <c r="K32" s="1">
@@ -4234,16 +4232,16 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1">
         <v>2009</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" s="1">
         <v>1367</v>
@@ -4252,19 +4250,19 @@
         <v>1449</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-82</v>
       </c>
       <c r="H33" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105.15384615384616</v>
       </c>
       <c r="I33" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111.46153846153847</v>
       </c>
       <c r="J33" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-6.3076923076923066</v>
       </c>
       <c r="K33" s="1">
@@ -4294,16 +4292,16 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1">
         <v>2010</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E34" s="1">
         <v>1707</v>
@@ -4312,19 +4310,19 @@
         <v>1421</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>286</v>
       </c>
       <c r="H34" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>131.30769230769232</v>
       </c>
       <c r="I34" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109.30769230769231</v>
       </c>
       <c r="J34" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22.000000000000014</v>
       </c>
       <c r="K34" s="1">
@@ -4354,16 +4352,16 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1">
         <v>2011</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E35" s="1">
         <v>1543</v>
@@ -4372,19 +4370,19 @@
         <v>1455</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" ref="G35:G40" si="8">E35-F35</f>
+        <f t="shared" ref="G35:G40" si="9">E35-F35</f>
         <v>88</v>
       </c>
       <c r="H35" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118.69230769230769</v>
       </c>
       <c r="I35" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111.92307692307692</v>
       </c>
       <c r="J35" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.7692307692307736</v>
       </c>
       <c r="K35" s="1">
@@ -4414,16 +4412,16 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="1">
         <v>2012</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E36" s="1">
         <v>1610</v>
@@ -4432,19 +4430,19 @@
         <v>1528</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>82</v>
       </c>
       <c r="H36" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123.84615384615384</v>
       </c>
       <c r="I36" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117.53846153846153</v>
       </c>
       <c r="J36" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.3076923076923066</v>
       </c>
       <c r="K36" s="1">
@@ -4474,16 +4472,16 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" s="1">
         <v>2013</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E37" s="1">
         <v>1573</v>
@@ -4492,19 +4490,19 @@
         <v>1667</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-94</v>
       </c>
       <c r="H37" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="I37" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>128.23076923076923</v>
       </c>
       <c r="J37" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7.2307692307692264</v>
       </c>
       <c r="K37" s="1">
@@ -4534,16 +4532,16 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1">
         <v>2014</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E38" s="1">
         <v>1601</v>
@@ -4552,19 +4550,19 @@
         <v>1460</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>141</v>
       </c>
       <c r="H38" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123.15384615384616</v>
       </c>
       <c r="I38" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>112.30769230769231</v>
       </c>
       <c r="J38" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.846153846153854</v>
       </c>
       <c r="K38" s="1">
@@ -4594,16 +4592,16 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1">
         <v>2015</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E39" s="1">
         <v>1654</v>
@@ -4612,19 +4610,19 @@
         <v>1844</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-190</v>
       </c>
       <c r="H39" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>127.23076923076923</v>
       </c>
       <c r="I39" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>141.84615384615384</v>
       </c>
       <c r="J39" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-14.615384615384613</v>
       </c>
       <c r="K39" s="1">
@@ -4654,16 +4652,16 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" s="1">
         <v>2016</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E40" s="1">
         <v>1613</v>
@@ -4672,19 +4670,19 @@
         <v>1594</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="H40" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124.07692307692308</v>
       </c>
       <c r="I40" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122.61538461538461</v>
       </c>
       <c r="J40" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.461538461538467</v>
       </c>
       <c r="K40" s="1">
@@ -4736,15 +4734,15 @@
         <v>134</v>
       </c>
       <c r="H41" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>81.941176470588232</v>
       </c>
       <c r="I41" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>74.058823529411768</v>
       </c>
       <c r="J41" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.8823529411764639</v>
       </c>
       <c r="K41" s="1">
@@ -4780,7 +4778,7 @@
         <v>2005</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>33</v>
@@ -4792,19 +4790,19 @@
         <v>1072</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" ref="G42:G47" si="9">E42-F42</f>
+        <f t="shared" ref="G42:G47" si="10">E42-F42</f>
         <v>-242</v>
       </c>
       <c r="H42" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63.846153846153847</v>
       </c>
       <c r="I42" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.461538461538467</v>
       </c>
       <c r="J42" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-18.61538461538462</v>
       </c>
       <c r="K42" s="1">
@@ -4852,19 +4850,19 @@
         <v>1316</v>
       </c>
       <c r="G43" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>41</v>
       </c>
       <c r="H43" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104.38461538461539</v>
       </c>
       <c r="I43" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101.23076923076923</v>
       </c>
       <c r="J43" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.1538461538461604</v>
       </c>
       <c r="K43" s="1">
@@ -4912,19 +4910,19 @@
         <v>1346</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>150</v>
       </c>
       <c r="H44" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115.07692307692308</v>
       </c>
       <c r="I44" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>103.53846153846153</v>
       </c>
       <c r="J44" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.538461538461547</v>
       </c>
       <c r="K44" s="1">
@@ -4960,10 +4958,10 @@
         <v>2008</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E45" s="1">
         <v>1447</v>
@@ -4972,19 +4970,19 @@
         <v>1365</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82</v>
       </c>
       <c r="H45" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111.30769230769231</v>
       </c>
       <c r="I45" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="J45" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.3076923076923066</v>
       </c>
       <c r="K45" s="1">
@@ -5020,10 +5018,10 @@
         <v>2009</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E46" s="1">
         <v>1442</v>
@@ -5032,19 +5030,19 @@
         <v>1447</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-5</v>
       </c>
       <c r="H46" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110.92307692307692</v>
       </c>
       <c r="I46" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111.30769230769231</v>
       </c>
       <c r="J46" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.3846153846153868</v>
       </c>
       <c r="K46" s="1">
@@ -5080,10 +5078,10 @@
         <v>2010</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E47" s="1">
         <v>1477</v>
@@ -5092,19 +5090,19 @@
         <v>1582</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-105</v>
       </c>
       <c r="H47" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113.61538461538461</v>
       </c>
       <c r="I47" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121.69230769230769</v>
       </c>
       <c r="J47" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-8.0769230769230802</v>
       </c>
       <c r="K47" s="1">
@@ -5140,10 +5138,10 @@
         <v>2011</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E48" s="1">
         <v>1600</v>
@@ -5152,19 +5150,19 @@
         <v>1590</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" ref="G48:G53" si="10">E48-F48</f>
+        <f t="shared" ref="G48:G53" si="11">E48-F48</f>
         <v>10</v>
       </c>
       <c r="H48" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123.07692307692308</v>
       </c>
       <c r="I48" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122.30769230769231</v>
       </c>
       <c r="J48" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7692307692307736</v>
       </c>
       <c r="K48" s="1">
@@ -5200,10 +5198,10 @@
         <v>2012</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="E49" s="1">
         <v>1665</v>
@@ -5212,19 +5210,19 @@
         <v>1437</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>228</v>
       </c>
       <c r="H49" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>128.07692307692307</v>
       </c>
       <c r="I49" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110.53846153846153</v>
       </c>
       <c r="J49" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17.538461538461533</v>
       </c>
       <c r="K49" s="1">
@@ -5260,10 +5258,10 @@
         <v>2013</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E50" s="1">
         <v>1541</v>
@@ -5272,19 +5270,19 @@
         <v>1572</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-31</v>
       </c>
       <c r="H50" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118.53846153846153</v>
       </c>
       <c r="I50" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120.92307692307692</v>
       </c>
       <c r="J50" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.3846153846153868</v>
       </c>
       <c r="K50" s="1">
@@ -5320,10 +5318,10 @@
         <v>2014</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E51" s="1">
         <v>1550</v>
@@ -5332,19 +5330,19 @@
         <v>1473</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>77</v>
       </c>
       <c r="H51" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119.23076923076923</v>
       </c>
       <c r="I51" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113.30769230769231</v>
       </c>
       <c r="J51" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.9230769230769198</v>
       </c>
       <c r="K51" s="1">
@@ -5380,10 +5378,10 @@
         <v>2015</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E52" s="1">
         <v>1427</v>
@@ -5392,19 +5390,19 @@
         <v>1531</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-104</v>
       </c>
       <c r="H52" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>109.76923076923077</v>
       </c>
       <c r="I52" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117.76923076923077</v>
       </c>
       <c r="J52" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-8</v>
       </c>
       <c r="K52" s="1">
@@ -5440,10 +5438,10 @@
         <v>2016</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E53" s="1">
         <v>1474</v>
@@ -5452,19 +5450,19 @@
         <v>1532</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-58</v>
       </c>
       <c r="H53" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113.38461538461539</v>
       </c>
       <c r="I53" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117.84615384615384</v>
       </c>
       <c r="J53" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.4615384615384528</v>
       </c>
       <c r="K53" s="1">
@@ -5516,15 +5514,15 @@
         <v>552</v>
       </c>
       <c r="H54" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>103.11764705882354</v>
       </c>
       <c r="I54" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70.647058823529406</v>
       </c>
       <c r="J54" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32.47058823529413</v>
       </c>
       <c r="K54" s="1">
@@ -5572,19 +5570,19 @@
         <v>1087</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" ref="G55:G60" si="11">E55-F55</f>
+        <f t="shared" ref="G55:G60" si="12">E55-F55</f>
         <v>-49</v>
       </c>
       <c r="H55" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>79.84615384615384</v>
       </c>
       <c r="I55" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.615384615384613</v>
       </c>
       <c r="J55" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3.7692307692307736</v>
       </c>
       <c r="K55" s="1">
@@ -5632,19 +5630,19 @@
         <v>1388</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-52</v>
       </c>
       <c r="H56" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102.76923076923077</v>
       </c>
       <c r="I56" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106.76923076923077</v>
       </c>
       <c r="J56" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
       <c r="K56" s="1">
@@ -5692,19 +5690,19 @@
         <v>1483</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-176</v>
       </c>
       <c r="H57" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100.53846153846153</v>
       </c>
       <c r="I57" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114.07692307692308</v>
       </c>
       <c r="J57" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-13.538461538461547</v>
       </c>
       <c r="K57" s="1">
@@ -5740,7 +5738,7 @@
         <v>2008</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>53</v>
@@ -5752,19 +5750,19 @@
         <v>1398</v>
       </c>
       <c r="G58" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-250</v>
       </c>
       <c r="H58" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>88.307692307692307</v>
       </c>
       <c r="I58" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>107.53846153846153</v>
       </c>
       <c r="J58" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-19.230769230769226</v>
       </c>
       <c r="K58" s="1">
@@ -5800,10 +5798,10 @@
         <v>2009</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E59" s="1">
         <v>1460</v>
@@ -5812,19 +5810,19 @@
         <v>1301</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>159</v>
       </c>
       <c r="H59" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>112.30769230769231</v>
       </c>
       <c r="I59" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100.07692307692308</v>
       </c>
       <c r="J59" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.230769230769226</v>
       </c>
       <c r="K59" s="1">
@@ -5860,10 +5858,10 @@
         <v>2010</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E60" s="1">
         <v>1378</v>
@@ -5872,19 +5870,19 @@
         <v>1499</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-121</v>
       </c>
       <c r="H60" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="I60" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115.30769230769231</v>
       </c>
       <c r="J60" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-9.3076923076923066</v>
       </c>
       <c r="K60" s="1">
@@ -5920,10 +5918,10 @@
         <v>2011</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E61" s="1">
         <v>1544</v>
@@ -5932,19 +5930,19 @@
         <v>1338</v>
       </c>
       <c r="G61" s="1">
-        <f t="shared" ref="G61:G66" si="12">E61-F61</f>
+        <f t="shared" ref="G61:G66" si="13">E61-F61</f>
         <v>206</v>
       </c>
       <c r="H61" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118.76923076923077</v>
       </c>
       <c r="I61" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102.92307692307692</v>
       </c>
       <c r="J61" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.846153846153854</v>
       </c>
       <c r="K61" s="1">
@@ -5983,7 +5981,7 @@
         <v>41</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E62" s="1">
         <v>1500</v>
@@ -5992,19 +5990,19 @@
         <v>1624</v>
       </c>
       <c r="G62" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-124</v>
       </c>
       <c r="H62" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115.38461538461539</v>
       </c>
       <c r="I62" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>124.92307692307692</v>
       </c>
       <c r="J62" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-9.538461538461533</v>
       </c>
       <c r="K62" s="1">
@@ -6040,10 +6038,10 @@
         <v>2013</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E63" s="1">
         <v>1572</v>
@@ -6052,19 +6050,19 @@
         <v>1474</v>
       </c>
       <c r="G63" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>98</v>
       </c>
       <c r="H63" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120.92307692307692</v>
       </c>
       <c r="I63" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113.38461538461539</v>
       </c>
       <c r="J63" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.538461538461533</v>
       </c>
       <c r="K63" s="1">
@@ -6100,10 +6098,10 @@
         <v>2014</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E64" s="1">
         <v>1706</v>
@@ -6112,19 +6110,19 @@
         <v>1580</v>
       </c>
       <c r="G64" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>126</v>
       </c>
       <c r="H64" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>131.23076923076923</v>
       </c>
       <c r="I64" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121.53846153846153</v>
       </c>
       <c r="J64" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.6923076923076934</v>
       </c>
       <c r="K64" s="1">
@@ -6160,10 +6158,10 @@
         <v>2015</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E65" s="1">
         <v>1696</v>
@@ -6172,19 +6170,19 @@
         <v>1440</v>
       </c>
       <c r="G65" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>256</v>
       </c>
       <c r="H65" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>130.46153846153845</v>
       </c>
       <c r="I65" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110.76923076923077</v>
       </c>
       <c r="J65" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19.692307692307679</v>
       </c>
       <c r="K65" s="1">
@@ -6220,10 +6218,10 @@
         <v>2016</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E66" s="1">
         <v>1667</v>
@@ -6232,19 +6230,19 @@
         <v>1558</v>
       </c>
       <c r="G66" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>109</v>
       </c>
       <c r="H66" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>128.23076923076923</v>
       </c>
       <c r="I66" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>119.84615384615384</v>
       </c>
       <c r="J66" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.3846153846153868</v>
       </c>
       <c r="K66" s="1">

</xml_diff>

<commit_message>
Revert "first branch test"
</commit_message>
<xml_diff>
--- a/FFData_Sep5.xlsx
+++ b/FFData_Sep5.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barkanir\Desktop\R\Scripts\FantasyFootballShinyDashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob&amp;Dev\Desktop\R\Scripts\FantasyFootballShinyDashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="League" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Top3Draft" sheetId="7" r:id="rId3"/>
     <sheet name="All" sheetId="9" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -614,7 +614,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1002,9 +1002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2300,7 +2298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>

</xml_diff>

<commit_message>
final commit sep 21 - proj almost done
</commit_message>
<xml_diff>
--- a/FFData_Sep5.xlsx
+++ b/FFData_Sep5.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob&amp;Dev\Desktop\R\Scripts\FantasyFootballShinyDashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barkanir\Desktop\R\Scripts\FantasyFootballShinyDashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="League" sheetId="1" r:id="rId1"/>
-    <sheet name="Top3Place" sheetId="8" r:id="rId2"/>
-    <sheet name="Top3Draft" sheetId="7" r:id="rId3"/>
-    <sheet name="All" sheetId="9" r:id="rId4"/>
+    <sheet name="Names" sheetId="10" r:id="rId2"/>
+    <sheet name="Top3Place" sheetId="8" r:id="rId3"/>
+    <sheet name="Top3Draft" sheetId="7" r:id="rId4"/>
+    <sheet name="All" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="237">
   <si>
     <t>Year</t>
   </si>
@@ -609,12 +610,141 @@
   </si>
   <si>
     <t>Top_3_Finsh</t>
+  </si>
+  <si>
+    <t>MiniW</t>
+  </si>
+  <si>
+    <t>DillyTheD</t>
+  </si>
+  <si>
+    <t>ConnorIsG</t>
+  </si>
+  <si>
+    <t>LickMyB</t>
+  </si>
+  <si>
+    <t>PunchinJ</t>
+  </si>
+  <si>
+    <t>TheBigHeadedJ</t>
+  </si>
+  <si>
+    <t>Sdonkeys</t>
+  </si>
+  <si>
+    <t>DonkeyPAH</t>
+  </si>
+  <si>
+    <t>PunchinMore J 06</t>
+  </si>
+  <si>
+    <t>MakesMyDookieSparkle</t>
+  </si>
+  <si>
+    <t>Pat Sajakin' B</t>
+  </si>
+  <si>
+    <t>J W D</t>
+  </si>
+  <si>
+    <t>Steamy Sweatin T&amp;T</t>
+  </si>
+  <si>
+    <t>Milf and Cookies</t>
+  </si>
+  <si>
+    <t>Foot Long Deuce</t>
+  </si>
+  <si>
+    <t>Bucco Blumpkin</t>
+  </si>
+  <si>
+    <t>Camel Towing</t>
+  </si>
+  <si>
+    <t>Big Pete's House of Munch</t>
+  </si>
+  <si>
+    <t>Pile Drivin T</t>
+  </si>
+  <si>
+    <t>Exploding Bo</t>
+  </si>
+  <si>
+    <t>4 Chicken Wings &amp; Rice</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Eric Karabell's C</t>
+  </si>
+  <si>
+    <t>3rd and Shlong</t>
+  </si>
+  <si>
+    <t>PurplDrankSlpryChank</t>
+  </si>
+  <si>
+    <t>SandusyATicklers</t>
+  </si>
+  <si>
+    <t>P and the B</t>
+  </si>
+  <si>
+    <t>Suck my V</t>
+  </si>
+  <si>
+    <t>Two Girls No Cutler</t>
+  </si>
+  <si>
+    <t>Don'tDieOnMeRalph</t>
+  </si>
+  <si>
+    <t>Squinty J</t>
+  </si>
+  <si>
+    <t>A Fister's</t>
+  </si>
+  <si>
+    <t>Mens As</t>
+  </si>
+  <si>
+    <t>MeetTheVanderSloots</t>
+  </si>
+  <si>
+    <t>Mouth Poo</t>
+  </si>
+  <si>
+    <t>Win'r Dine'r 49er</t>
+  </si>
+  <si>
+    <t>Carlos Danger</t>
+  </si>
+  <si>
+    <t>Golen Taint</t>
+  </si>
+  <si>
+    <t>Cosby's Sleepers</t>
+  </si>
+  <si>
+    <t>TrumpsAnchorBaby</t>
+  </si>
+  <si>
+    <t>Turd McButt Face</t>
+  </si>
+  <si>
+    <t>LowIQMika</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1002,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1257,6 +1387,525 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B56"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2">
+        <f ca="1">ROUNDUP(RANDBETWEEN(1,5),0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B56" ca="1" si="0">ROUNDUP(RANDBETWEEN(1,5),0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>204</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>207</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>209</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>210</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>211</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>212</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>213</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>214</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>217</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>218</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>219</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>220</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>221</v>
+      </c>
+      <c r="B36">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>222</v>
+      </c>
+      <c r="B37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>224</v>
+      </c>
+      <c r="B39">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>225</v>
+      </c>
+      <c r="B40">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>226</v>
+      </c>
+      <c r="B41">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>227</v>
+      </c>
+      <c r="B43">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>228</v>
+      </c>
+      <c r="B44">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>229</v>
+      </c>
+      <c r="B45">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>230</v>
+      </c>
+      <c r="B46">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>231</v>
+      </c>
+      <c r="B47">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>232</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>161</v>
+      </c>
+      <c r="B50">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>233</v>
+      </c>
+      <c r="B51">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>234</v>
+      </c>
+      <c r="B52">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>235</v>
+      </c>
+      <c r="B55">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>236</v>
+      </c>
+      <c r="B56">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
@@ -1835,11 +2484,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2294,13 +2943,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>